<commit_message>
Mega commit (3 commits que viraram 1 so)
</commit_message>
<xml_diff>
--- a/me262.xlsx
+++ b/me262.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CEFET\8o Periodo\Computacao Grafica\CG-Tp1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Visual Studio 2013\Projects\CG-Tp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -133,9 +133,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -173,7 +173,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -245,7 +245,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O67"/>
+  <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54:K65"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J85" sqref="J85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,11 +814,11 @@
         <v>7</v>
       </c>
       <c r="M16">
-        <f>I12/18.5</f>
+        <f t="shared" ref="M16:N21" si="3">I12/18.5</f>
         <v>0.2810810810810811</v>
       </c>
       <c r="N16">
-        <f>J12/18.5</f>
+        <f t="shared" si="3"/>
         <v>0.23783783783783785</v>
       </c>
     </row>
@@ -844,11 +844,11 @@
         <v>3.7</v>
       </c>
       <c r="M17">
-        <f>I13/18.5</f>
+        <f t="shared" si="3"/>
         <v>0.2810810810810811</v>
       </c>
       <c r="N17">
-        <f>J13/18.5</f>
+        <f t="shared" si="3"/>
         <v>0.3783783783783784</v>
       </c>
     </row>
@@ -871,11 +871,11 @@
         <v>1</v>
       </c>
       <c r="M18">
-        <f>I14/18.5</f>
+        <f t="shared" si="3"/>
         <v>0.30270270270270266</v>
       </c>
       <c r="N18">
-        <f>J14/18.5</f>
+        <f t="shared" si="3"/>
         <v>0.44864864864864867</v>
       </c>
     </row>
@@ -904,11 +904,11 @@
         <v>78</v>
       </c>
       <c r="M19">
-        <f>I15/18.5</f>
+        <f t="shared" si="3"/>
         <v>0.3783783783783784</v>
       </c>
       <c r="N19">
-        <f>J15/18.5</f>
+        <f t="shared" si="3"/>
         <v>0.44864864864864867</v>
       </c>
     </row>
@@ -926,11 +926,11 @@
         <v>6</v>
       </c>
       <c r="M20">
-        <f>I16/18.5</f>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
       <c r="N20">
-        <f>J16/18.5</f>
+        <f t="shared" si="3"/>
         <v>0.3783783783783784</v>
       </c>
     </row>
@@ -957,11 +957,11 @@
         <v>-1.9</v>
       </c>
       <c r="M21">
-        <f>I17/18.5</f>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
       <c r="N21">
-        <f>J17/18.5</f>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
     </row>
@@ -996,11 +996,11 @@
         <v>-3</v>
       </c>
       <c r="M23">
-        <f>I21/18.5</f>
+        <f t="shared" ref="M23:N26" si="4">I21/18.5</f>
         <v>0.2864864864864865</v>
       </c>
       <c r="N23">
-        <f>J21/18.5</f>
+        <f t="shared" si="4"/>
         <v>-0.10270270270270269</v>
       </c>
     </row>
@@ -1018,11 +1018,11 @@
         <v>-1.5</v>
       </c>
       <c r="M24">
-        <f>I22/18.5</f>
+        <f t="shared" si="4"/>
         <v>0.30270270270270266</v>
       </c>
       <c r="N24">
-        <f>J22/18.5</f>
+        <f t="shared" si="4"/>
         <v>-0.16216216216216217</v>
       </c>
     </row>
@@ -1034,11 +1034,11 @@
         <v>-0.16216216216216217</v>
       </c>
       <c r="M25">
-        <f>I23/18.5</f>
+        <f t="shared" si="4"/>
         <v>0.3783783783783784</v>
       </c>
       <c r="N25">
-        <f>J23/18.5</f>
+        <f t="shared" si="4"/>
         <v>-0.16216216216216217</v>
       </c>
     </row>
@@ -1050,11 +1050,11 @@
         <v>-0.10810810810810811</v>
       </c>
       <c r="M26">
-        <f>I24/18.5</f>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="N26">
-        <f>J24/18.5</f>
+        <f t="shared" si="4"/>
         <v>-8.1081081081081086E-2</v>
       </c>
     </row>
@@ -1251,11 +1251,11 @@
         <v>0.36078431372549019</v>
       </c>
       <c r="F38">
-        <f t="shared" ref="F38:G38" si="3">B21/255</f>
+        <f t="shared" ref="F38:G38" si="5">B21/255</f>
         <v>0.35686274509803922</v>
       </c>
       <c r="G38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.38039215686274508</v>
       </c>
       <c r="I38">
@@ -1431,203 +1431,203 @@
     </row>
     <row r="55" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J55">
-        <f t="shared" ref="J55:J65" si="4">-I35/18.5</f>
+        <f t="shared" ref="J55:J65" si="6">-I35/18.5</f>
         <v>-0.25945945945945947</v>
       </c>
       <c r="K55">
-        <f t="shared" ref="K55:K65" si="5">J35/18.5</f>
+        <f t="shared" ref="K55:K65" si="7">J35/18.5</f>
         <v>9.7297297297297303E-2</v>
       </c>
       <c r="M55">
-        <f t="shared" ref="M55:N55" si="6">I35/18.5</f>
+        <f t="shared" ref="M55:N55" si="8">I35/18.5</f>
         <v>0.25945945945945947</v>
       </c>
       <c r="N55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>9.7297297297297303E-2</v>
       </c>
     </row>
     <row r="56" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.25945945945945947</v>
       </c>
       <c r="K56">
-        <f t="shared" si="5"/>
-        <v>0.16216216216216217</v>
-      </c>
-      <c r="M56">
-        <f t="shared" ref="M56:N56" si="7">I36/18.5</f>
-        <v>0.25945945945945947</v>
-      </c>
-      <c r="N56">
         <f t="shared" si="7"/>
         <v>0.16216216216216217</v>
       </c>
+      <c r="M56">
+        <f t="shared" ref="M56:N56" si="9">I36/18.5</f>
+        <v>0.25945945945945947</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="9"/>
+        <v>0.16216216216216217</v>
+      </c>
     </row>
     <row r="57" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.22702702702702704</v>
       </c>
       <c r="K57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.16216216216216217</v>
       </c>
       <c r="M57">
-        <f t="shared" ref="M57:N57" si="8">I37/18.5</f>
+        <f t="shared" ref="M57:N57" si="10">I37/18.5</f>
         <v>0.22702702702702704</v>
       </c>
       <c r="N57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.16216216216216217</v>
       </c>
     </row>
     <row r="58" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.22702702702702704</v>
       </c>
       <c r="K58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.7297297297297303E-2</v>
       </c>
       <c r="M58">
-        <f t="shared" ref="M58:N58" si="9">I38/18.5</f>
+        <f t="shared" ref="M58:N58" si="11">I38/18.5</f>
         <v>0.22702702702702704</v>
       </c>
       <c r="N58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>9.7297297297297303E-2</v>
       </c>
     </row>
     <row r="59" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.16216216216216217</v>
       </c>
       <c r="K59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.7297297297297303E-2</v>
       </c>
       <c r="M59">
-        <f t="shared" ref="M59:N59" si="10">I39/18.5</f>
+        <f t="shared" ref="M59:N59" si="12">I39/18.5</f>
         <v>0.16216216216216217</v>
       </c>
       <c r="N59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>9.7297297297297303E-2</v>
       </c>
     </row>
     <row r="60" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.16216216216216217</v>
       </c>
       <c r="K60">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.4864864864864868E-2</v>
       </c>
       <c r="M60">
-        <f t="shared" ref="M60:N60" si="11">I40/18.5</f>
+        <f t="shared" ref="M60:N60" si="13">I40/18.5</f>
         <v>0.16216216216216217</v>
       </c>
       <c r="N60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6.4864864864864868E-2</v>
       </c>
     </row>
     <row r="61" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.22702702702702704</v>
       </c>
       <c r="K61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.4864864864864868E-2</v>
       </c>
       <c r="M61">
-        <f t="shared" ref="M61:N61" si="12">I41/18.5</f>
+        <f t="shared" ref="M61:N61" si="14">I41/18.5</f>
         <v>0.22702702702702704</v>
       </c>
       <c r="N61">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>6.4864864864864868E-2</v>
       </c>
     </row>
     <row r="62" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J62">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.22702702702702704</v>
       </c>
       <c r="K62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M62">
-        <f t="shared" ref="M62:N62" si="13">I42/18.5</f>
+        <f t="shared" ref="M62:N62" si="15">I42/18.5</f>
         <v>0.22702702702702704</v>
       </c>
       <c r="N62">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J63">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.25945945945945947</v>
       </c>
       <c r="K63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M63">
-        <f t="shared" ref="M63:N63" si="14">I43/18.5</f>
+        <f t="shared" ref="M63:N63" si="16">I43/18.5</f>
         <v>0.25945945945945947</v>
       </c>
       <c r="N63">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.25945945945945947</v>
       </c>
       <c r="K64">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.4864864864864868E-2</v>
       </c>
       <c r="M64">
-        <f t="shared" ref="M64:N64" si="15">I44/18.5</f>
+        <f t="shared" ref="M64:N64" si="17">I44/18.5</f>
         <v>0.25945945945945947</v>
       </c>
       <c r="N64">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6.4864864864864868E-2</v>
       </c>
     </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.32432432432432434</v>
       </c>
       <c r="K65">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.4864864864864868E-2</v>
       </c>
       <c r="M65">
-        <f t="shared" ref="M65:N65" si="16">I45/18.5</f>
+        <f t="shared" ref="M65:N65" si="18">I45/18.5</f>
         <v>0.32432432432432434</v>
       </c>
       <c r="N65">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>6.4864864864864868E-2</v>
       </c>
     </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J66" t="s">
         <v>1</v>
       </c>
@@ -1635,12 +1635,374 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J67" t="s">
         <v>12</v>
       </c>
       <c r="M67" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>-0.32432432432432434</v>
+      </c>
+      <c r="C69">
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="E69">
+        <v>-0.32432432432432434</v>
+      </c>
+      <c r="F69">
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="G69">
+        <f>10000*E69</f>
+        <v>-3243.2432432432433</v>
+      </c>
+      <c r="H69">
+        <f>10000*F69</f>
+        <v>972.97297297297303</v>
+      </c>
+    </row>
+    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>-0.25945945945945947</v>
+      </c>
+      <c r="C70">
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="E70">
+        <v>-0.25945945945945947</v>
+      </c>
+      <c r="F70">
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="G70">
+        <f t="shared" ref="G70:G77" si="19">10000*E70</f>
+        <v>-2594.5945945945946</v>
+      </c>
+      <c r="H70">
+        <f t="shared" ref="H70:H77" si="20">10000*F70</f>
+        <v>972.97297297297303</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>-0.25945945945945947</v>
+      </c>
+      <c r="C71">
+        <v>0.16216216216216217</v>
+      </c>
+      <c r="E71">
+        <v>-0.22702702702702704</v>
+      </c>
+      <c r="F71">
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="19"/>
+        <v>-2270.2702702702704</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="20"/>
+        <v>972.97297297297303</v>
+      </c>
+    </row>
+    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>-0.22702702702702704</v>
+      </c>
+      <c r="C72">
+        <v>0.16216216216216217</v>
+      </c>
+      <c r="E72">
+        <v>-0.16216216216216217</v>
+      </c>
+      <c r="F72">
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="19"/>
+        <v>-1621.6216216216217</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="20"/>
+        <v>972.97297297297303</v>
+      </c>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>-0.22702702702702704</v>
+      </c>
+      <c r="C73">
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="E73">
+        <v>-0.16216216216216217</v>
+      </c>
+      <c r="F73">
+        <v>6.4864864864864868E-2</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="19"/>
+        <v>-1621.6216216216217</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="20"/>
+        <v>648.64864864864865</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>-0.16216216216216217</v>
+      </c>
+      <c r="C74">
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="E74">
+        <v>-0.22702702702702704</v>
+      </c>
+      <c r="F74">
+        <v>6.4864864864864868E-2</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="19"/>
+        <v>-2270.2702702702704</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="20"/>
+        <v>648.64864864864865</v>
+      </c>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>-0.16216216216216217</v>
+      </c>
+      <c r="C75">
+        <v>6.4864864864864868E-2</v>
+      </c>
+      <c r="E75">
+        <v>-0.25945945945945947</v>
+      </c>
+      <c r="F75">
+        <v>6.4864864864864868E-2</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="19"/>
+        <v>-2594.5945945945946</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="20"/>
+        <v>648.64864864864865</v>
+      </c>
+    </row>
+    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>-0.22702702702702704</v>
+      </c>
+      <c r="C76">
+        <v>6.4864864864864868E-2</v>
+      </c>
+      <c r="E76">
+        <v>-0.32432432432432434</v>
+      </c>
+      <c r="F76">
+        <v>6.4864864864864868E-2</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="19"/>
+        <v>-3243.2432432432433</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="20"/>
+        <v>648.64864864864865</v>
+      </c>
+    </row>
+    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>-0.22702702702702704</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>-0.32432432432432434</v>
+      </c>
+      <c r="F77">
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="19"/>
+        <v>-3243.2432432432433</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="20"/>
+        <v>972.97297297297303</v>
+      </c>
+    </row>
+    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>-0.25945945945945947</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>-0.25945945945945947</v>
+      </c>
+      <c r="C79">
+        <v>6.4864864864864868E-2</v>
+      </c>
+      <c r="E79">
+        <v>-0.25945945945945947</v>
+      </c>
+      <c r="F79">
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="G79">
+        <f>10000*E79</f>
+        <v>-2594.5945945945946</v>
+      </c>
+      <c r="H79">
+        <f>10000*F79</f>
+        <v>972.97297297297303</v>
+      </c>
+    </row>
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>-0.32432432432432434</v>
+      </c>
+      <c r="C80">
+        <v>6.4864864864864868E-2</v>
+      </c>
+      <c r="E80">
+        <v>-0.25945945945945947</v>
+      </c>
+      <c r="F80">
+        <v>0.16216216216216217</v>
+      </c>
+      <c r="G80">
+        <f t="shared" ref="G80:G87" si="21">10000*E80</f>
+        <v>-2594.5945945945946</v>
+      </c>
+      <c r="H80">
+        <f t="shared" ref="H80:H87" si="22">10000*F80</f>
+        <v>1621.6216216216217</v>
+      </c>
+    </row>
+    <row r="81" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>-0.22702702702702704</v>
+      </c>
+      <c r="F81">
+        <v>0.16216216216216217</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="21"/>
+        <v>-2270.2702702702704</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="22"/>
+        <v>1621.6216216216217</v>
+      </c>
+    </row>
+    <row r="82" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>-0.22702702702702704</v>
+      </c>
+      <c r="F82">
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="21"/>
+        <v>-2270.2702702702704</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="22"/>
+        <v>972.97297297297303</v>
+      </c>
+    </row>
+    <row r="83" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>-0.22702702702702704</v>
+      </c>
+      <c r="F83">
+        <v>6.4864864864864868E-2</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="21"/>
+        <v>-2270.2702702702704</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="22"/>
+        <v>648.64864864864865</v>
+      </c>
+    </row>
+    <row r="84" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>-0.22702702702702704</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="21"/>
+        <v>-2270.2702702702704</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>-0.25945945945945947</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="21"/>
+        <v>-2594.5945945945946</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>-0.25945945945945947</v>
+      </c>
+      <c r="F86">
+        <v>6.4864864864864868E-2</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="21"/>
+        <v>-2594.5945945945946</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="22"/>
+        <v>648.64864864864865</v>
+      </c>
+    </row>
+    <row r="87" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>-0.25945945945945947</v>
+      </c>
+      <c r="F87">
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="21"/>
+        <v>-2594.5945945945946</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="22"/>
+        <v>972.97297297297303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>